<commit_message>
modify the checkitem table's fk
</commit_message>
<xml_diff>
--- a/ocms_database_design_draft.xlsx
+++ b/ocms_database_design_draft.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16800" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="projects" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="60">
   <si>
     <t>カラム名</t>
     <rPh sb="3" eb="4">
@@ -84,10 +84,6 @@
   </si>
   <si>
     <t>ci_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>fk</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -328,14 +324,14 @@
     <t>関連ゴール</t>
   </si>
   <si>
-    <t>ファーザーID</t>
+    <t>引用表checkitemのci_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,14 +342,6 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
@@ -423,692 +411,698 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="229">
+  <cellStyleXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1125,10 +1119,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -1138,7 +1132,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="229">
+  <cellStyles count="231">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1253,6 +1247,7 @@
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1367,6 +1362,7 @@
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1671,7 +1667,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1707,16 +1703,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17">
@@ -1724,13 +1720,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1741,10 +1737,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1792,56 +1788,56 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1894,56 +1890,56 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="17">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1986,43 +1982,43 @@
     </row>
     <row r="2" spans="1:4" ht="17">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="17">
       <c r="A3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="17">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="17">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2039,25 +2035,25 @@
     </row>
     <row r="8" spans="1:4" ht="17">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="17">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -2078,13 +2074,14 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2101,63 +2098,65 @@
     </row>
     <row r="2" spans="1:4" ht="17">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="17">
       <c r="A3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="17">
       <c r="A4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="17">
       <c r="A5" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="17">
       <c r="A6" s="4" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2200,117 +2199,117 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="3"/>
     </row>

</xml_diff>

<commit_message>
foreign key restriction is modified.
</commit_message>
<xml_diff>
--- a/ocms_database_design_draft.xlsx
+++ b/ocms_database_design_draft.xlsx
@@ -1,38 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuich\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6980" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="4" r:id="rId1"/>
     <sheet name="checklist" sheetId="3" r:id="rId2"/>
     <sheet name="item" sheetId="2" r:id="rId3"/>
-    <sheet name="item_checkitem" sheetId="5" r:id="rId4"/>
-    <sheet name="checkitem" sheetId="1" r:id="rId5"/>
-    <sheet name="checkitem_status" sheetId="6" r:id="rId6"/>
+    <sheet name="item_checkitem_status" sheetId="5" r:id="rId4"/>
+    <sheet name="checkitem_status" sheetId="6" r:id="rId5"/>
+    <sheet name="checkitem" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
   <si>
     <t>カラム名</t>
     <rPh sb="3" eb="4">
@@ -90,7 +85,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="游ゴシック"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -129,58 +124,608 @@
     <t>チェックリスト名</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
+    <t>checkitem_status_id</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>状態</t>
+  </si>
+  <si>
+    <t>コメント</t>
+  </si>
+  <si>
+    <t>成果物</t>
+  </si>
+  <si>
+    <t>重要度</t>
+  </si>
+  <si>
+    <t>補充説明</t>
+  </si>
+  <si>
+    <t>変更履歴</t>
+  </si>
+  <si>
+    <t>不遵守事項有無</t>
+  </si>
+  <si>
+    <t>項目内容</t>
+  </si>
+  <si>
+    <t>関連項目</t>
+  </si>
+  <si>
+    <t>関連ゴール</t>
+  </si>
+  <si>
+    <t>checklist_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>percentage</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>percentage</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>related_goal_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>related_item_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>comment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>deliverables</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>prjtype</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>importance</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>history</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>problem</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>checkitem_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>item_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>item_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>checklist_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>project_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>project_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>parent_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>prj_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>主キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、自</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>動採</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>番、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>外部キー、引用表</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>checklist</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
+      <t>not null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>、外部キー</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t>名</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="游ゴシック"/>
+      <t>unsigned</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、引用表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
-      <t>fk_items_</t>
+      <t>checklist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>名</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fk_items_checklist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unsigned</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>。外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>制限</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">On update cascade, On delete cascase </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>引用表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、参照列</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>item_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>名：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fk_items_item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unsigned</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>。外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>制限</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>On update cascade, On delete cascade</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、引用表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>、外部キ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Lantinghei SC Demibold"/>
+        <family val="2"/>
+      </rPr>
+      <t>ー</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Libian SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t>名</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fk_checklists_project</t>
     </r>
     <r>
       <rPr>
@@ -190,173 +735,68 @@
         <family val="2"/>
         <charset val="128"/>
       </rPr>
-      <t>checklist</t>
-    </r>
-  </si>
-  <si>
-    <t>checkitem_status_id</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>状態</t>
-  </si>
-  <si>
-    <t>コメント</t>
-  </si>
-  <si>
-    <t>成果物</t>
-  </si>
-  <si>
-    <t>重要度</t>
-  </si>
-  <si>
-    <t>補充説明</t>
-  </si>
-  <si>
-    <t>変更履歴</t>
-  </si>
-  <si>
-    <t>不遵守事項有無</t>
-  </si>
-  <si>
-    <t>項目内容</t>
-  </si>
-  <si>
-    <t>関連項目</t>
-  </si>
-  <si>
-    <t>関連ゴール</t>
-  </si>
-  <si>
-    <t>checklist_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>percentage</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>percentage</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>related_goal_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>related_item_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>comment</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>deliverables</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>prjtype</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>importance</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>history</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>problem</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="1"/>
+      <t>。not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>外部キー、引用表item、外部キー名fk_item_checklists_item、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>外部キー、引用表checkitem_status、外部キー名fk_item_checklists_checkitem_status、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
+    </r>
   </si>
   <si>
     <t>checkitem_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>checkitem_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>item_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>item_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>checklist_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>project_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>project_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>引用表itemのitm_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>parent_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>外部キー、引用表project、外部キー名fk_checklists_project</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>prj_id</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>外部キー、引用表checkitem、外部キー名fk_chekitem_statuses_checkitem、not null、unsigned。外部キー制限On update cascade, On delete cascade</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -365,7 +805,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -374,7 +814,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -392,6 +832,20 @@
       <name val="Libian SC Regular"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lantinghei SC Demibold"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -401,7 +855,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -425,18 +879,29 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="231">
+  <cellStyleXfs count="325">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1130,8 +1595,290 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1147,260 +1894,360 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="231">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="185" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="187" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="189" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="191" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="193" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="195" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="197" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="199" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="201" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="203" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="205" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="207" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="209" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="211" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="213" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="215" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="217" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="219" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="221" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="223" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="225" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="227" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="229" builtinId="8" hidden="1"/>
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="228" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="230" builtinId="9" hidden="1"/>
+  <cellStyles count="325">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1704,7 +2551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1714,11 +2561,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
@@ -1743,7 +2590,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -1752,12 +2599,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="17">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -1771,7 +2618,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1797,18 +2644,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.58203125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1823,18 +2670,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="17">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1842,7 +2689,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -1856,29 +2703,38 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:4" ht="57">
+      <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>58</v>
+      <c r="D5" s="12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="B6" s="8"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -1896,18 +2752,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="48" style="7" customWidth="1"/>
-    <col min="5" max="5" width="23" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="7"/>
+    <col min="1" max="1" width="11.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="53.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="23" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1927,7 +2783,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
@@ -1941,7 +2797,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -1955,39 +2811,39 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="48">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" customFormat="1">
-      <c r="A6" s="4" t="s">
+      <c r="D5" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>56</v>
+      <c r="D6" s="13" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2007,13 +2863,16 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="6"/>
+    <col min="4" max="4" width="72.33203125" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2029,61 +2888,64 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
+      <c r="D3" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="5"/>
+      <c r="D4" s="13" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2099,17 +2961,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="6"/>
+    <col min="4" max="4" width="79" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2125,56 +2989,128 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" ht="28">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D11" s="13" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2186,17 +3122,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="7" customWidth="1"/>
-    <col min="2" max="2" width="17" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="14" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="6"/>
+    <col min="4" max="4" width="33.1640625" style="6" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2216,121 +3154,55 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>